<commit_message>
Added 12-pin and 4-pin spring terminal footprints. Updated footprints for ADC board. Continued work on PCB layout of ADC board.
</commit_message>
<xml_diff>
--- a/Orders.xlsx
+++ b/Orders.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Documents\GitHub\SDAQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F14A0F5B-7826-4FC8-B5FD-96C0BE9AB2D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC86738-8AFD-471C-90AF-901F824F49C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mouser Order" sheetId="1" r:id="rId1"/>
@@ -567,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -685,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66BC5D1B-4CB4-4F44-8D0B-13A0EAE44CA5}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Actually moved the csv into the Orders sheet
</commit_message>
<xml_diff>
--- a/Orders.xlsx
+++ b/Orders.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Documents\GitHub\SDAQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC86738-8AFD-471C-90AF-901F824F49C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C25A1C-1051-41C5-9D18-68C8BBF19E7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mouser Order" sheetId="1" r:id="rId1"/>
-    <sheet name="Digikey Order" sheetId="3" r:id="rId2"/>
-    <sheet name="Amazon Order" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId2"/>
+    <sheet name="Digikey Order" sheetId="3" r:id="rId3"/>
+    <sheet name="Amazon Order" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -104,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="91">
   <si>
     <t>Part #</t>
   </si>
@@ -224,6 +225,159 @@
   </si>
   <si>
     <t>SAM1204-10-ND</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Part Number</t>
+  </si>
+  <si>
+    <t>Manufacturer Part Number</t>
+  </si>
+  <si>
+    <t>Customer Reference</t>
+  </si>
+  <si>
+    <t>Available</t>
+  </si>
+  <si>
+    <t>Backorder</t>
+  </si>
+  <si>
+    <t>Unit Price</t>
+  </si>
+  <si>
+    <t>Extended Price USD</t>
+  </si>
+  <si>
+    <t>563-CFS-0102CT-ND</t>
+  </si>
+  <si>
+    <t>CFS-0102TB</t>
+  </si>
+  <si>
+    <t>SWITCH DIP 1POS SPST 100MA 6V</t>
+  </si>
+  <si>
+    <t>490-CSTNE16M0V53L000R0CT-ND</t>
+  </si>
+  <si>
+    <t>CSTNE16M0V53L000R0</t>
+  </si>
+  <si>
+    <t>3.2X1.3MM 16.0MHZ CERAMIC RESONA</t>
+  </si>
+  <si>
+    <t>LT1117CST-5#TRPBFCT-ND</t>
+  </si>
+  <si>
+    <t>LT1117CST-5#TRPBF</t>
+  </si>
+  <si>
+    <t>IC REG LINEAR 5V 800MA SOT223-3</t>
+  </si>
+  <si>
+    <t>TSW-103-14-F-S</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 3POS 2.54MM</t>
+  </si>
+  <si>
+    <t>QPC02SXGN-RC</t>
+  </si>
+  <si>
+    <t>CONN JUMPER SHORTING .100" GOLD</t>
+  </si>
+  <si>
+    <t>277-5744-ND</t>
+  </si>
+  <si>
+    <t>TERM BLK 4POS SIDE ENT 3.5MM PCB</t>
+  </si>
+  <si>
+    <t>Z2929-ND</t>
+  </si>
+  <si>
+    <t>G5Q-14 DC5</t>
+  </si>
+  <si>
+    <t>RELAY GEN PURPOSE SPDT 10A 5V</t>
+  </si>
+  <si>
+    <t>SAM11096-ND</t>
+  </si>
+  <si>
+    <t>ESQ-110-13-L-D</t>
+  </si>
+  <si>
+    <t>CONN SOCKET 20POS 0.1 GOLD PCB</t>
+  </si>
+  <si>
+    <t>ESQ-120-13-T-D-ND</t>
+  </si>
+  <si>
+    <t>ESQ-120-13-T-D</t>
+  </si>
+  <si>
+    <t>CONN SOCKET 40POS 0.1 TIN PCB</t>
+  </si>
+  <si>
+    <t>SSQ-112-03-T-D</t>
+  </si>
+  <si>
+    <t>CONN RCPT 24POS 0.1 TIN PCB</t>
+  </si>
+  <si>
+    <t>SAM11124-ND</t>
+  </si>
+  <si>
+    <t>ESW-105-12-L-D</t>
+  </si>
+  <si>
+    <t>CONN SOCKET 10POS 0.1 GOLD PCB</t>
+  </si>
+  <si>
+    <t>609-77313-127-10LF-ND</t>
+  </si>
+  <si>
+    <t>77313-127-10LF</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 10POS 2.54MM</t>
+  </si>
+  <si>
+    <t>S2212EC-03-ND</t>
+  </si>
+  <si>
+    <t>PREC003DFAN-RC</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 6POS 2.54MM</t>
+  </si>
+  <si>
+    <t>296-52901-ND</t>
+  </si>
+  <si>
+    <t>LM358DG4</t>
+  </si>
+  <si>
+    <t>IC OPAMP GP 2 CIRCUIT 8SOIC</t>
+  </si>
+  <si>
+    <t>BCS-103-T-D-TE-ND</t>
+  </si>
+  <si>
+    <t>BCS-103-T-D-TE</t>
+  </si>
+  <si>
+    <t>CONN RCPT 6POS 0.1 TIN PCB</t>
+  </si>
+  <si>
+    <t>1195-6406-ND</t>
+  </si>
+  <si>
+    <t>CBL 3POS MALE TO FMALE 16.4'</t>
   </si>
 </sst>
 </file>
@@ -567,7 +721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -682,6 +836,517 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8C8442F-0CF2-48C6-8CC5-91ADD7E9365D}">
+  <dimension ref="A1:J17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="J2">
+        <v>7.74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="J3">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>5.1719999999999997</v>
+      </c>
+      <c r="J4">
+        <v>51.72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5">
+        <v>50</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="J5">
+        <v>19.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6">
+        <v>30</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>4.0800000000000003E-2</v>
+      </c>
+      <c r="J6">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7">
+        <v>1751264</v>
+      </c>
+      <c r="E7" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7">
+        <v>30</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>2.7490000000000001</v>
+      </c>
+      <c r="J7">
+        <v>82.47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8">
+        <v>13</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>1.556</v>
+      </c>
+      <c r="J8">
+        <v>20.23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9">
+        <v>10</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>6.01</v>
+      </c>
+      <c r="J9">
+        <v>60.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" t="s">
+        <v>71</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>7.64</v>
+      </c>
+      <c r="J10">
+        <v>38.200000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11">
+        <v>8</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>2.56</v>
+      </c>
+      <c r="J11">
+        <v>20.48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" t="s">
+        <v>76</v>
+      </c>
+      <c r="G12">
+        <v>7</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>2.99</v>
+      </c>
+      <c r="J12">
+        <v>20.93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" t="s">
+        <v>79</v>
+      </c>
+      <c r="G13">
+        <v>7</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0.62</v>
+      </c>
+      <c r="J13">
+        <v>4.34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" t="s">
+        <v>82</v>
+      </c>
+      <c r="G14">
+        <v>7</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0.16</v>
+      </c>
+      <c r="J14">
+        <v>1.1200000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" t="s">
+        <v>84</v>
+      </c>
+      <c r="E15" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15">
+        <v>20</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0.879</v>
+      </c>
+      <c r="J15">
+        <v>17.579999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>86</v>
+      </c>
+      <c r="D16" t="s">
+        <v>87</v>
+      </c>
+      <c r="E16" t="s">
+        <v>88</v>
+      </c>
+      <c r="G16">
+        <v>7</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>1.84</v>
+      </c>
+      <c r="J16">
+        <v>12.88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17">
+        <v>21348081380050</v>
+      </c>
+      <c r="E17" t="s">
+        <v>90</v>
+      </c>
+      <c r="G17">
+        <v>10</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>14.282999999999999</v>
+      </c>
+      <c r="J17">
+        <v>142.83000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66BC5D1B-4CB4-4F44-8D0B-13A0EAE44CA5}">
   <dimension ref="A1:I12"/>
   <sheetViews>
@@ -929,7 +1594,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{117A3385-D7F1-4F71-92B1-0498F124BCF5}">
   <dimension ref="A1:H9"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updated order sheet name
</commit_message>
<xml_diff>
--- a/Orders.xlsx
+++ b/Orders.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Documents\GitHub\SDAQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C25A1C-1051-41C5-9D18-68C8BBF19E7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C639887-B376-40D5-AC4F-4CACCC8F6891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mouser Order" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId2"/>
+    <sheet name="March 26 Order" sheetId="6" r:id="rId2"/>
     <sheet name="Digikey Order" sheetId="3" r:id="rId3"/>
     <sheet name="Amazon Order" sheetId="5" r:id="rId4"/>
   </sheets>
@@ -840,7 +840,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="E21" sqref="E19:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>